<commit_message>
Se añade PKS-DDS y complementa PKS-GEDI
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A228ED49-79FD-42A8-99A6-FA1411F9B686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EE4C48-71A3-46B9-8004-F07720830D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +460,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7B7B7"/>
         <bgColor rgb="FFB7B7B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -577,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -653,16 +659,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -683,6 +679,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,7 +918,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -923,15 +935,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -966,7 +978,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
@@ -981,7 +993,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="37" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="1"/>
@@ -998,7 +1010,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="39">
+      <c r="J5" s="33">
         <v>44480</v>
       </c>
       <c r="K5" s="1"/>
@@ -1015,7 +1027,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="40">
+      <c r="J6" s="34">
         <v>44487</v>
       </c>
       <c r="K6" s="1"/>
@@ -1032,7 +1044,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="41">
+      <c r="J7" s="35">
         <v>44494</v>
       </c>
       <c r="K7" s="1"/>
@@ -1047,7 +1059,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="36" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
@@ -1075,7 +1087,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="36" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="1"/>
@@ -1103,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="J10" s="41">
+      <c r="J10" s="35">
         <v>44515</v>
       </c>
       <c r="K10" s="1"/>
@@ -1112,7 +1124,7 @@
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="46" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1131,16 +1143,16 @@
         <v>0</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="J11" s="41">
+      <c r="J11" s="35">
         <v>44522</v>
       </c>
-      <c r="K11" s="35"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="46" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1159,10 +1171,10 @@
         <v>0</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="J12" s="41">
+      <c r="J12" s="35">
         <v>44529</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="30" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1189,16 +1201,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="45" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1214,13 +1226,13 @@
         <v>44499</v>
       </c>
       <c r="G14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="J14" s="41">
+      <c r="J14" s="35">
         <v>44543</v>
       </c>
-      <c r="K14" s="35"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="17" t="s">
@@ -1245,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="J15" s="41">
+      <c r="J15" s="35">
         <v>44550</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1275,19 +1287,19 @@
         <v>0</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="J16" s="41">
+      <c r="J16" s="35">
         <v>44557</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="38" t="s">
         <v>106</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -1300,13 +1312,13 @@
         <v>44502</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="15">
       <c r="A18" s="13" t="s">
@@ -1327,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="J18" s="41">
+      <c r="J18" s="35">
         <v>44571</v>
       </c>
-      <c r="K18" s="37" t="s">
+      <c r="K18" s="31" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1349,10 +1361,10 @@
       </c>
       <c r="G19" s="23"/>
       <c r="H19" s="1"/>
-      <c r="J19" s="41">
+      <c r="J19" s="35">
         <v>44578</v>
       </c>
-      <c r="K19" s="35"/>
+      <c r="K19" s="29"/>
     </row>
     <row r="20" spans="1:11" ht="15">
       <c r="A20" s="9" t="s">
@@ -1377,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="J20" s="41">
+      <c r="J20" s="35">
         <v>44585</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="30" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1779,22 +1791,22 @@
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:4" ht="14.25">
+      <c r="A1" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="27" t="s">
         <v>83</v>
       </c>
@@ -1803,10 +1815,10 @@
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="28" t="s">
         <v>86</v>
       </c>
@@ -1815,10 +1827,10 @@
       <c r="A4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="28" t="s">
         <v>89</v>
       </c>
@@ -1827,10 +1839,10 @@
       <c r="A5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="28" t="s">
         <v>92</v>
       </c>
@@ -1839,10 +1851,10 @@
       <c r="A6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="28" t="s">
         <v>95</v>
       </c>
@@ -1851,10 +1863,10 @@
       <c r="A7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="2" t="s">
         <v>92</v>
       </c>
@@ -1863,10 +1875,10 @@
       <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="2" t="s">
         <v>100</v>
       </c>
@@ -1875,10 +1887,10 @@
       <c r="A9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="2" t="s">
         <v>103</v>
       </c>
@@ -1887,10 +1899,10 @@
       <c r="A10" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="28" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Agregado historias de usuario
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Proyecto GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLEGA3\Desktop\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EE4C48-71A3-46B9-8004-F07720830D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F62924-E9F5-4731-AD03-9410E3B177A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23295" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -130,15 +130,9 @@
     <t>Parcial</t>
   </si>
   <si>
-    <t>Listado Historias de Usuario</t>
-  </si>
-  <si>
     <t>Documento de Historias de Usuario</t>
   </si>
   <si>
-    <t>PKS-DHU.XLSX</t>
-  </si>
-  <si>
     <t>Cordova /A</t>
   </si>
   <si>
@@ -359,6 +353,12 @@
   </si>
   <si>
     <t>https://github.com/julianntorres/GCS-G3</t>
+  </si>
+  <si>
+    <t>Historias de Usuario</t>
+  </si>
+  <si>
+    <t>PKS-DHU.DOCX</t>
   </si>
 </sst>
 </file>
@@ -681,6 +681,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,12 +697,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -935,15 +935,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -954,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1124,7 +1124,7 @@
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="40" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1149,10 +1149,10 @@
       <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="40" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1180,16 +1180,16 @@
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="E13" s="15">
         <v>44496</v>
@@ -1202,22 +1202,22 @@
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="1:11" ht="15">
+      <c r="A14" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="45" t="s">
+      <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="D14" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="E14" s="16">
         <v>44498</v>
@@ -1236,16 +1236,16 @@
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="D15" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>44</v>
       </c>
       <c r="E15" s="19">
         <v>44499</v>
@@ -1261,21 +1261,21 @@
         <v>44550</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E16" s="10">
         <v>44499</v>
@@ -1294,16 +1294,16 @@
     </row>
     <row r="17" spans="1:11" ht="15">
       <c r="A17" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="38" t="s">
-        <v>107</v>
-      </c>
       <c r="C17" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="10">
         <v>44500</v>
@@ -1316,16 +1316,16 @@
       </c>
       <c r="H17" s="1"/>
       <c r="J17" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="15">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1343,12 +1343,12 @@
         <v>44571</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15">
       <c r="A19" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -1368,16 +1368,16 @@
     </row>
     <row r="20" spans="1:11" ht="15">
       <c r="A20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="E20" s="24">
         <v>44506</v>
@@ -1393,21 +1393,21 @@
         <v>44585</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15">
       <c r="A21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="E21" s="24">
         <v>44514</v>
@@ -1423,10 +1423,10 @@
     </row>
     <row r="22" spans="1:11" ht="15">
       <c r="A22" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="23" spans="1:11" ht="15">
       <c r="A23" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -1463,16 +1463,16 @@
     </row>
     <row r="24" spans="1:11" ht="15">
       <c r="A24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E24" s="24">
         <v>44526</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="25" spans="1:11" ht="15">
       <c r="A25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E25" s="24">
         <v>44900</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="26" spans="1:11" ht="15">
       <c r="A26" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="D26" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="E26" s="24">
         <v>44542</v>
@@ -1541,16 +1541,16 @@
     </row>
     <row r="27" spans="1:11" ht="15">
       <c r="A27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="D27" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="E27" s="24">
         <v>44542</v>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="28" spans="1:11" ht="15">
       <c r="A28" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="29" spans="1:11" ht="15">
       <c r="A29" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -1792,119 +1792,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25">
-      <c r="A1" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="44"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="27" t="s">
         <v>81</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="27" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="28" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="28" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="28" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="28" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="42"/>
+        <v>94</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="44"/>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="42"/>
+        <v>102</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="44"/>
       <c r="D10" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reubicación de archivos y marcado en cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOLEGA3\Desktop\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GIT GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A037516-5CCB-4E81-9586-87B832594E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F85E32-6061-4E4F-98F8-36167066A8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23295" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -917,8 +917,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1140,7 +1140,7 @@
         <v>44496</v>
       </c>
       <c r="G11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="35">
@@ -1168,7 +1168,7 @@
         <v>44500</v>
       </c>
       <c r="G12" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="35">

</xml_diff>

<commit_message>
se actualiza PKS-C y el plan de gestión - actividad semana 9
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main\CASILLEROS\Alexis\UNMSM\2021 - 2\Cursos\Configuracion de SW\Proyecto\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GIT GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE559688-4DC9-4070-A89B-890C41145B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
     <sheet name="Roles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -363,7 +353,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -906,14 +896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1279,7 +1269,7 @@
         <v>44502</v>
       </c>
       <c r="G16" s="12">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="34">
@@ -1331,7 +1321,7 @@
         <v>44505</v>
       </c>
       <c r="G18" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1"/>
       <c r="J18" s="34">
@@ -1354,7 +1344,9 @@
       <c r="F19" s="21">
         <v>44505</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="22">
+        <v>1</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="J19" s="34">
         <v>44578</v>
@@ -1381,7 +1373,7 @@
         <v>44513</v>
       </c>
       <c r="G20" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="34">
@@ -1411,7 +1403,7 @@
         <v>44551</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1432,7 +1424,7 @@
         <v>44523</v>
       </c>
       <c r="G22" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1451,7 +1443,9 @@
       <c r="F23" s="25">
         <v>44523</v>
       </c>
-      <c r="G23" s="22"/>
+      <c r="G23" s="22">
+        <v>1</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1476,7 +1470,7 @@
         <v>44534</v>
       </c>
       <c r="G24" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1502,7 +1496,7 @@
         <v>44542</v>
       </c>
       <c r="G25" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1771,7 +1765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>

<commit_message>
Conformación líneas base 1 y 2 - reestructuración de módulos en PKS-C
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GIT GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE559688-4DC9-4070-A89B-890C41145B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDCF32-4C99-4E44-BA94-7088863D3B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37785" yWindow="960" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Reyes /A</t>
+  </si>
+  <si>
+    <t>31/11/2021</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,12 +451,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB7B7B7"/>
         <bgColor rgb="FFB7B7B7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -571,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -594,24 +591,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,12 +604,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,9 +648,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,6 +658,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,7 +888,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -920,15 +905,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -963,7 +948,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="28"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
@@ -978,7 +963,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="30" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="1"/>
@@ -995,7 +980,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="32">
+      <c r="J5" s="26">
         <v>44480</v>
       </c>
       <c r="K5" s="1"/>
@@ -1012,7 +997,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="33">
+      <c r="J6" s="27">
         <v>44487</v>
       </c>
       <c r="K6" s="1"/>
@@ -1029,7 +1014,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="34">
+      <c r="J7" s="28">
         <v>44494</v>
       </c>
       <c r="K7" s="1"/>
@@ -1044,7 +1029,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="29" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
@@ -1072,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="29" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="1"/>
@@ -1090,26 +1075,26 @@
       <c r="D10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="12">
         <v>44486</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="12">
         <v>44491</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <v>1</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="J10" s="34">
+      <c r="J10" s="28">
         <v>44515</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1118,26 +1103,26 @@
       <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="10">
-        <v>44494</v>
-      </c>
-      <c r="F11" s="14">
-        <v>44496</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="E11" s="12">
+        <v>44492</v>
+      </c>
+      <c r="F11" s="12">
+        <v>44495</v>
+      </c>
+      <c r="G11" s="10">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="J11" s="34">
+      <c r="J11" s="28">
         <v>44522</v>
       </c>
-      <c r="K11" s="28"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="32" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1146,28 +1131,28 @@
       <c r="D12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>44496</v>
       </c>
-      <c r="F12" s="10">
-        <v>44500</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="F12" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="10">
         <v>1</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="J12" s="34">
+      <c r="J12" s="28">
         <v>44529</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1176,26 +1161,26 @@
       <c r="D13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="15">
-        <v>44496</v>
-      </c>
-      <c r="F13" s="10">
-        <v>44500</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="E13" s="12">
+        <v>44502</v>
+      </c>
+      <c r="F13" s="12">
+        <v>44506</v>
+      </c>
+      <c r="G13" s="10">
         <v>1</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="32" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1204,48 +1189,48 @@
       <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="16">
-        <v>44498</v>
-      </c>
-      <c r="F14" s="16">
-        <v>44499</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="E14" s="12">
+        <v>44502</v>
+      </c>
+      <c r="F14" s="12">
+        <v>44506</v>
+      </c>
+      <c r="G14" s="10">
         <v>1</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="J14" s="34">
+      <c r="J14" s="28">
         <v>44543</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="19">
-        <v>44499</v>
-      </c>
-      <c r="F15" s="19">
-        <v>44502</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="E15" s="12">
+        <v>44507</v>
+      </c>
+      <c r="F15" s="12">
+        <v>44509</v>
+      </c>
+      <c r="G15" s="10">
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="J15" s="34">
+      <c r="J15" s="28">
         <v>44550</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1253,7 +1238,7 @@
       <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1262,103 +1247,103 @@
       <c r="D16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="10">
-        <v>44499</v>
-      </c>
-      <c r="F16" s="19">
-        <v>44502</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="E16" s="12">
+        <v>44509</v>
+      </c>
+      <c r="F16" s="12">
+        <v>44511</v>
+      </c>
+      <c r="G16" s="10">
         <v>1</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="J16" s="34">
+      <c r="J16" s="28">
         <v>44557</v>
       </c>
-      <c r="K16" s="31"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="31" t="s">
         <v>103</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="10">
-        <v>44500</v>
-      </c>
-      <c r="F17" s="16">
-        <v>44502</v>
-      </c>
-      <c r="G17" s="12">
+      <c r="E17" s="12">
+        <v>44476</v>
+      </c>
+      <c r="F17" s="12">
+        <v>44511</v>
+      </c>
+      <c r="G17" s="10">
         <v>1</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="J17" s="35" t="s">
+      <c r="J17" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="28"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="16">
-        <v>44502</v>
-      </c>
-      <c r="F18" s="16">
-        <v>44505</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12">
+        <v>44512</v>
+      </c>
+      <c r="F18" s="12">
+        <v>44512</v>
+      </c>
+      <c r="G18" s="10">
         <v>1</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="J18" s="34">
+      <c r="J18" s="28">
         <v>44571</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="K18" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="15">
         <v>44486</v>
       </c>
-      <c r="F19" s="21">
-        <v>44505</v>
-      </c>
-      <c r="G19" s="22">
+      <c r="F19" s="15">
+        <v>44512</v>
+      </c>
+      <c r="G19" s="16">
         <v>1</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="J19" s="34">
+      <c r="J19" s="28">
         <v>44578</v>
       </c>
-      <c r="K19" s="28"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" ht="15">
-      <c r="A20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>54</v>
+      <c r="A20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>55</v>
@@ -1366,20 +1351,20 @@
       <c r="D20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="23">
-        <v>44506</v>
-      </c>
-      <c r="F20" s="23">
+      <c r="E20" s="17">
         <v>44513</v>
       </c>
-      <c r="G20" s="12">
+      <c r="F20" s="17">
+        <v>44520</v>
+      </c>
+      <c r="G20" s="10">
         <v>1</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="J20" s="34">
+      <c r="J20" s="28">
         <v>44585</v>
       </c>
-      <c r="K20" s="29" t="s">
+      <c r="K20" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1396,34 +1381,34 @@
       <c r="D21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="23">
-        <v>44514</v>
-      </c>
-      <c r="F21" s="23">
-        <v>44551</v>
-      </c>
-      <c r="G21" s="12">
+      <c r="E21" s="17">
+        <v>44521</v>
+      </c>
+      <c r="F21" s="17">
+        <v>44558</v>
+      </c>
+      <c r="G21" s="10">
         <v>1</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="15">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="23">
-        <v>44521</v>
-      </c>
-      <c r="F22" s="23">
-        <v>44523</v>
-      </c>
-      <c r="G22" s="12">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="17">
+        <v>44529</v>
+      </c>
+      <c r="F22" s="17">
+        <v>44529</v>
+      </c>
+      <c r="G22" s="10">
         <v>1</v>
       </c>
       <c r="H22" s="1"/>
@@ -1431,19 +1416,19 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="15">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="24">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="18">
         <v>44506</v>
       </c>
-      <c r="F23" s="25">
-        <v>44523</v>
-      </c>
-      <c r="G23" s="22">
+      <c r="F23" s="19">
+        <v>44529</v>
+      </c>
+      <c r="G23" s="16">
         <v>1</v>
       </c>
       <c r="H23" s="1"/>
@@ -1451,11 +1436,11 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="15">
-      <c r="A24" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>63</v>
+      <c r="A24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>64</v>
@@ -1463,13 +1448,13 @@
       <c r="D24" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="23">
-        <v>44526</v>
-      </c>
-      <c r="F24" s="23">
-        <v>44534</v>
-      </c>
-      <c r="G24" s="12">
+      <c r="E24" s="17">
+        <v>44529</v>
+      </c>
+      <c r="F24" s="17">
+        <v>44537</v>
+      </c>
+      <c r="G24" s="10">
         <v>1</v>
       </c>
       <c r="H24" s="1"/>
@@ -1489,13 +1474,13 @@
       <c r="D25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="23">
-        <v>44900</v>
-      </c>
-      <c r="F25" s="23">
-        <v>44542</v>
-      </c>
-      <c r="G25" s="12">
+      <c r="E25" s="17">
+        <v>44903</v>
+      </c>
+      <c r="F25" s="17">
+        <v>44545</v>
+      </c>
+      <c r="G25" s="10">
         <v>0.3</v>
       </c>
       <c r="H25" s="1"/>
@@ -1503,10 +1488,10 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="15">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -1515,13 +1500,13 @@
       <c r="D26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="23">
-        <v>44542</v>
-      </c>
-      <c r="F26" s="23">
+      <c r="E26" s="17">
+        <v>44545</v>
+      </c>
+      <c r="F26" s="17">
         <v>44548</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="10">
         <v>0</v>
       </c>
       <c r="H26" s="1"/>
@@ -1529,10 +1514,10 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="15">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -1541,13 +1526,13 @@
       <c r="D27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="23">
-        <v>44542</v>
-      </c>
-      <c r="F27" s="23">
+      <c r="E27" s="17">
+        <v>44545</v>
+      </c>
+      <c r="F27" s="17">
         <v>44548</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="10">
         <v>0</v>
       </c>
       <c r="H27" s="1"/>
@@ -1555,21 +1540,21 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="15">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="23">
-        <v>44549</v>
-      </c>
-      <c r="F28" s="23">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="17">
+        <v>44545</v>
+      </c>
+      <c r="F28" s="17">
         <v>44550</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="10">
         <v>0</v>
       </c>
       <c r="H28" s="1"/>
@@ -1577,19 +1562,19 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="25">
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="19">
         <v>44526</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="19">
         <v>44550</v>
       </c>
-      <c r="G29" s="22"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1607,8 +1592,6 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1688,10 +1671,21 @@
       <c r="K39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G18">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1702,7 +1696,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G22">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1710,8 +1706,6 @@
         <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1728,14 +1722,6 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="5" tint="0.39997558519241921"/>
-        <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1781,22 +1767,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="26" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="20" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1804,11 +1790,11 @@
       <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="21" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1816,11 +1802,11 @@
       <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="27" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1828,11 +1814,11 @@
       <c r="A5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="27" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="21" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1840,11 +1826,11 @@
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="21" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1852,10 +1838,10 @@
       <c r="A7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="2" t="s">
         <v>89</v>
       </c>
@@ -1864,10 +1850,10 @@
       <c r="A8" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="2" t="s">
         <v>97</v>
       </c>
@@ -1876,10 +1862,10 @@
       <c r="A9" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="2" t="s">
         <v>100</v>
       </c>
@@ -1888,11 +1874,11 @@
       <c r="A10" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="21" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentación líneas base 1 y 2
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GIT GCSW\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEDCF32-4C99-4E44-BA94-7088863D3B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DE6CE3-DCD2-4B62-9BF5-1AB393B70842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37785" yWindow="960" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23250" yWindow="-1095" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="119">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -89,9 +89,6 @@
     <t>PKS-C.XLSX</t>
   </si>
   <si>
-    <t>Tumi / DS</t>
-  </si>
-  <si>
     <t>Reunión con el Cliente</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>PKS-DR.DOCX</t>
   </si>
   <si>
-    <t>Paredes /JP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elaboración del documento de arquitectura </t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>PKS-PP.DOCX</t>
   </si>
   <si>
-    <t>Torres /DB, Tumi/DS , Paredes /JP</t>
-  </si>
-  <si>
     <t>Parcial</t>
   </si>
   <si>
@@ -351,6 +342,42 @@
   </si>
   <si>
     <t>31/11/2021</t>
+  </si>
+  <si>
+    <t>Domumentación de Línea Base 1</t>
+  </si>
+  <si>
+    <t>Domumentación de Línea Base 2</t>
+  </si>
+  <si>
+    <t>PKS-DLB1.DOCX</t>
+  </si>
+  <si>
+    <t>Tumi/JP</t>
+  </si>
+  <si>
+    <t>Paredes /DB</t>
+  </si>
+  <si>
+    <t>Torres /DB, Tumi/JP , Paredes /DB</t>
+  </si>
+  <si>
+    <t>Domumentación de Línea Base 3</t>
+  </si>
+  <si>
+    <t>PKS-DLB2.DOCX</t>
+  </si>
+  <si>
+    <t>PKS-DLB3.DOCX</t>
+  </si>
+  <si>
+    <t>Periodo de ejecución del Sprint 1</t>
+  </si>
+  <si>
+    <t>Periodo de ejecución del Sprint 2</t>
+  </si>
+  <si>
+    <t>Periodo de ejecución del Sprint 3</t>
   </si>
 </sst>
 </file>
@@ -410,7 +437,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,8 +480,14 @@
         <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -564,11 +597,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -606,16 +707,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,13 +753,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,10 +1019,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -905,15 +1039,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -924,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -948,7 +1082,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
@@ -963,7 +1097,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="28" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="1"/>
@@ -980,7 +1114,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="26">
+      <c r="J5" s="24">
         <v>44480</v>
       </c>
       <c r="K5" s="1"/>
@@ -997,7 +1131,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="27">
+      <c r="J6" s="25">
         <v>44487</v>
       </c>
       <c r="K6" s="1"/>
@@ -1014,7 +1148,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="28">
+      <c r="J7" s="26">
         <v>44494</v>
       </c>
       <c r="K7" s="1"/>
@@ -1029,7 +1163,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="27" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
@@ -1057,7 +1191,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="1"/>
@@ -1073,7 +1207,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="E10" s="12">
         <v>44486</v>
@@ -1085,23 +1219,23 @@
         <v>1</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="J10" s="28">
+      <c r="J10" s="26">
         <v>44515</v>
       </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="C11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="9" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="E11" s="12">
         <v>44492</v>
@@ -1113,53 +1247,53 @@
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="J11" s="28">
+      <c r="J11" s="26">
         <v>44522</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="E12" s="12">
         <v>44496</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="J12" s="28">
+      <c r="J12" s="26">
         <v>44529</v>
       </c>
-      <c r="K12" s="23" t="s">
-        <v>31</v>
+      <c r="K12" s="21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E13" s="12">
         <v>44502</v>
@@ -1171,23 +1305,23 @@
         <v>1</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="15">
+      <c r="A14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="22"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="32" t="s">
+      <c r="D14" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="E14" s="12">
         <v>44502</v>
@@ -1199,23 +1333,23 @@
         <v>1</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="J14" s="28">
+      <c r="J14" s="26">
         <v>44543</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="E15" s="12">
         <v>44507</v>
@@ -1227,25 +1361,25 @@
         <v>1</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="J15" s="28">
+      <c r="J15" s="26">
         <v>44550</v>
       </c>
-      <c r="K15" s="24" t="s">
-        <v>42</v>
+      <c r="K15" s="22" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="E16" s="12">
         <v>44509</v>
@@ -1257,23 +1391,23 @@
         <v>1</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="J16" s="28">
+      <c r="J16" s="26">
         <v>44557</v>
       </c>
-      <c r="K16" s="25"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>103</v>
+      <c r="A17" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" s="12">
         <v>44476</v>
@@ -1285,150 +1419,152 @@
         <v>1</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" ht="15">
+      <c r="A18" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12">
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="46">
         <v>44512</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="46">
         <v>44512</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="J18" s="28">
+      <c r="J18" s="26">
         <v>44571</v>
       </c>
-      <c r="K18" s="24" t="s">
+      <c r="K18" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15">
+      <c r="A19" s="42" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="15">
+      <c r="B19" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="52">
+        <v>44475</v>
+      </c>
+      <c r="F19" s="52">
+        <v>44512</v>
+      </c>
+      <c r="G19" s="45">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="J19" s="26">
+        <v>44578</v>
+      </c>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" ht="15">
+      <c r="A20" s="43"/>
+      <c r="B20" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50">
         <v>44486</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F20" s="51">
         <v>44512</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G20" s="15">
         <v>1</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="J19" s="28">
-        <v>44578</v>
-      </c>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:11" ht="15">
-      <c r="A20" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="17">
+      <c r="H20" s="1"/>
+      <c r="J20" s="26">
+        <v>44585</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15">
+      <c r="A21" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="37">
         <v>44513</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F21" s="16">
         <v>44520</v>
-      </c>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="J20" s="28">
-        <v>44585</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15">
-      <c r="A21" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="17">
-        <v>44521</v>
-      </c>
-      <c r="F21" s="17">
-        <v>44558</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="15">
-      <c r="A22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="17">
-        <v>44529</v>
-      </c>
-      <c r="F22" s="17">
-        <v>44529</v>
+      <c r="A22" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="37">
+        <v>44521</v>
+      </c>
+      <c r="F22" s="16">
+        <v>44528</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="15">
-      <c r="A23" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
+      <c r="A23" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="41"/>
       <c r="D23" s="41"/>
-      <c r="E23" s="18">
-        <v>44506</v>
-      </c>
-      <c r="F23" s="19">
+      <c r="E23" s="37">
         <v>44529</v>
       </c>
-      <c r="G23" s="16">
+      <c r="F23" s="16">
+        <v>44529</v>
+      </c>
+      <c r="G23" s="10">
         <v>1</v>
       </c>
       <c r="H23" s="1"/>
@@ -1436,23 +1572,21 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="15">
-      <c r="A24" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="17">
+      <c r="A24" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="52">
+        <v>44521</v>
+      </c>
+      <c r="F24" s="52">
         <v>44529</v>
-      </c>
-      <c r="F24" s="17">
-        <v>44537</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -1462,97 +1596,95 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="15">
-      <c r="A25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="17">
-        <v>44903</v>
+      <c r="A25" s="43"/>
+      <c r="B25" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="38">
+        <v>44506</v>
       </c>
       <c r="F25" s="17">
-        <v>44545</v>
-      </c>
-      <c r="G25" s="10">
-        <v>0.3</v>
+        <v>44529</v>
+      </c>
+      <c r="G25" s="15">
+        <v>1</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="15">
-      <c r="A26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="17">
-        <v>44545</v>
-      </c>
-      <c r="F26" s="17">
-        <v>44548</v>
+      <c r="A26" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="37">
+        <v>44529</v>
+      </c>
+      <c r="F26" s="16">
+        <v>44537</v>
       </c>
       <c r="G26" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="15">
-      <c r="A27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="17">
+      <c r="A27" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="37">
+        <v>44903</v>
+      </c>
+      <c r="F27" s="16">
         <v>44545</v>
       </c>
-      <c r="F27" s="17">
-        <v>44548</v>
-      </c>
       <c r="G27" s="10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="15">
-      <c r="A28" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="17">
+      <c r="A28" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="37">
         <v>44545</v>
       </c>
-      <c r="F28" s="17">
-        <v>44550</v>
+      <c r="F28" s="16">
+        <v>44548</v>
       </c>
       <c r="G28" s="10">
         <v>0</v>
@@ -1562,61 +1694,109 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15">
-      <c r="A29" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="19">
-        <v>44526</v>
-      </c>
-      <c r="F29" s="19">
-        <v>44550</v>
-      </c>
-      <c r="G29" s="16"/>
+      <c r="A29" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="37">
+        <v>44545</v>
+      </c>
+      <c r="F29" s="16">
+        <v>44548</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="15">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="A30" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="37">
+        <v>44545</v>
+      </c>
+      <c r="F30" s="16">
+        <v>44550</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="15">
-      <c r="C31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="44"/>
+      <c r="E31" s="52">
+        <v>44537</v>
+      </c>
+      <c r="F31" s="52">
+        <v>44550</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="15">
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="39">
+        <v>44526</v>
+      </c>
+      <c r="F32" s="17">
+        <v>44550</v>
+      </c>
+      <c r="G32" s="15"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="5:11" ht="15">
+    </row>
+    <row r="33" spans="1:11" ht="15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="5:11" ht="15">
+    <row r="34" spans="1:11" ht="15">
+      <c r="C34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1625,7 +1805,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="5:11" ht="15">
+    <row r="35" spans="1:11" ht="15">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1634,16 +1814,13 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="5:11" ht="15">
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+    <row r="36" spans="1:11" ht="15">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="5:11" ht="15">
+    <row r="37" spans="1:11" ht="15">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1652,7 +1829,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="5:11" ht="15">
+    <row r="38" spans="1:11" ht="15">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1661,7 +1838,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="5:11" ht="15">
+    <row r="39" spans="1:11" ht="15">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1670,14 +1847,44 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
+    <row r="40" spans="1:11" ht="15">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" ht="15">
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" ht="15">
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
-  <conditionalFormatting sqref="G10:G18">
+  <conditionalFormatting sqref="G10:G19">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1697,7 +1904,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G22">
+  <conditionalFormatting sqref="G21:G24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1725,7 +1932,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1735,7 +1942,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G28">
+  <conditionalFormatting sqref="G26:G31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>
@@ -1757,7 +1964,9 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1767,119 +1976,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="21" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="21" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="21" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="19" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="19" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="36"/>
+        <v>90</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="34"/>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="36"/>
+        <v>92</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="34"/>
       <c r="D8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="36"/>
+        <v>95</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="34"/>
       <c r="D9" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="19" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadiendo manual - Empleado-S-B
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main\CASILLEROS\Alexis\UNMSM\2021 - 2\Cursos\Configuracion de SW\Proyecto\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\Desktop\CICLO  VI - 2021-II\Gestion de la Configuracion del Software\Proyecto\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE7385-2A95-4CF1-8EE5-D5C088858A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="5760" yWindow="1716" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -382,7 +383,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -1014,27 +1015,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="5" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
@@ -1281,7 +1282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" ht="14.4">
       <c r="A13" s="11" t="s">
         <v>103</v>
       </c>
@@ -1309,7 +1310,7 @@
       </c>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" ht="14.4">
       <c r="A14" s="30" t="s">
         <v>31</v>
       </c>
@@ -1337,7 +1338,7 @@
       </c>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" ht="14.4">
       <c r="A15" s="13" t="s">
         <v>35</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" ht="14.4">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -1395,7 +1396,7 @@
       </c>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" ht="14.4">
       <c r="A17" s="29" t="s">
         <v>99</v>
       </c>
@@ -1423,7 +1424,7 @@
       </c>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" ht="14.4">
       <c r="A18" s="34" t="s">
         <v>46</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" ht="14.4">
       <c r="A19" s="45" t="s">
         <v>48</v>
       </c>
@@ -1475,7 +1476,7 @@
       </c>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" ht="14.4">
       <c r="A20" s="46"/>
       <c r="B20" s="42" t="s">
         <v>116</v>
@@ -1499,7 +1500,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" ht="14.4">
       <c r="A21" s="35" t="s">
         <v>59</v>
       </c>
@@ -1523,7 +1524,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" ht="14.4">
       <c r="A22" s="35" t="s">
         <v>54</v>
       </c>
@@ -1548,7 +1549,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="15">
+    <row r="23" spans="1:11" ht="14.4">
       <c r="A23" s="35" t="s">
         <v>46</v>
       </c>
@@ -1570,7 +1571,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="15">
+    <row r="24" spans="1:11" ht="14.4">
       <c r="A24" s="45" t="s">
         <v>58</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="15">
+    <row r="25" spans="1:11" ht="14.4">
       <c r="A25" s="46"/>
       <c r="B25" s="42" t="s">
         <v>117</v>
@@ -1614,7 +1615,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="15">
+    <row r="26" spans="1:11" ht="14.4">
       <c r="A26" s="35" t="s">
         <v>50</v>
       </c>
@@ -1640,7 +1641,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="15">
+    <row r="27" spans="1:11" ht="14.4">
       <c r="A27" s="35" t="s">
         <v>62</v>
       </c>
@@ -1666,7 +1667,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="15">
+    <row r="28" spans="1:11" ht="14.4">
       <c r="A28" s="35" t="s">
         <v>65</v>
       </c>
@@ -1692,7 +1693,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="15">
+    <row r="29" spans="1:11" ht="14.4">
       <c r="A29" s="35" t="s">
         <v>69</v>
       </c>
@@ -1718,7 +1719,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="15">
+    <row r="30" spans="1:11" ht="14.4">
       <c r="A30" s="35" t="s">
         <v>46</v>
       </c>
@@ -1734,13 +1735,13 @@
         <v>44550</v>
       </c>
       <c r="G30" s="10">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="15">
+    <row r="31" spans="1:11" ht="14.4">
       <c r="A31" s="45" t="s">
         <v>73</v>
       </c>
@@ -1764,7 +1765,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="15">
+    <row r="32" spans="1:11" ht="14.4">
       <c r="A32" s="46"/>
       <c r="B32" s="42" t="s">
         <v>118</v>
@@ -1782,7 +1783,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="15">
+    <row r="33" spans="1:11" ht="14.4">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1794,7 +1795,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="15">
+    <row r="34" spans="1:11" ht="14.4">
       <c r="C34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1804,7 +1805,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="15">
+    <row r="35" spans="1:11" ht="14.4">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1813,13 +1814,13 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="15">
+    <row r="36" spans="1:11" ht="14.4">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="15">
+    <row r="37" spans="1:11" ht="14.4">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1828,7 +1829,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="15">
+    <row r="38" spans="1:11" ht="14.4">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1837,7 +1838,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="15">
+    <row r="39" spans="1:11" ht="14.4">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1846,7 +1847,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="15">
+    <row r="40" spans="1:11" ht="14.4">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1855,7 +1856,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="15">
+    <row r="41" spans="1:11" ht="14.4">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1864,7 +1865,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="15">
+    <row r="42" spans="1:11" ht="14.4">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1957,7 +1958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1967,14 +1968,14 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25">
+    <row r="1" spans="1:4" ht="13.8">
       <c r="A1" s="51" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Manual de usuario - Admin añadido
</commit_message>
<xml_diff>
--- a/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
+++ b/Desarrollo/Parking Soft/Gestión/PKS-C.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm\Desktop\CICLO  VI - 2021-II\Gestion de la Configuracion del Software\Proyecto\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main\CASILLEROS\Alexis\UNMSM\2021 - 2\Cursos\Configuracion de SW\Proyecto\GCS-G3\Desarrollo\Parking Soft\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE7385-2A95-4CF1-8EE5-D5C088858A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1716" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1710" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -383,7 +382,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
@@ -1015,27 +1014,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
-    <col min="5" max="6" width="11.33203125" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
@@ -1282,7 +1281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.4">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="11" t="s">
         <v>103</v>
       </c>
@@ -1310,7 +1309,7 @@
       </c>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="30" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1337,7 @@
       </c>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" ht="14.4">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="13" t="s">
         <v>35</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.4">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -1396,7 +1395,7 @@
       </c>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" ht="14.4">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="29" t="s">
         <v>99</v>
       </c>
@@ -1424,7 +1423,7 @@
       </c>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" ht="14.4">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="34" t="s">
         <v>46</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.4">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="45" t="s">
         <v>48</v>
       </c>
@@ -1476,7 +1475,7 @@
       </c>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" ht="14.4">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="46"/>
       <c r="B20" s="42" t="s">
         <v>116</v>
@@ -1500,7 +1499,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.4">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="35" t="s">
         <v>59</v>
       </c>
@@ -1524,7 +1523,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="14.4">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="35" t="s">
         <v>54</v>
       </c>
@@ -1549,7 +1548,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="14.4">
+    <row r="23" spans="1:11" ht="15">
       <c r="A23" s="35" t="s">
         <v>46</v>
       </c>
@@ -1571,7 +1570,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="14.4">
+    <row r="24" spans="1:11" ht="15">
       <c r="A24" s="45" t="s">
         <v>58</v>
       </c>
@@ -1595,7 +1594,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="14.4">
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="46"/>
       <c r="B25" s="42" t="s">
         <v>117</v>
@@ -1615,7 +1614,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="14.4">
+    <row r="26" spans="1:11" ht="15">
       <c r="A26" s="35" t="s">
         <v>50</v>
       </c>
@@ -1641,7 +1640,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="14.4">
+    <row r="27" spans="1:11" ht="15">
       <c r="A27" s="35" t="s">
         <v>62</v>
       </c>
@@ -1667,7 +1666,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="14.4">
+    <row r="28" spans="1:11" ht="15">
       <c r="A28" s="35" t="s">
         <v>65</v>
       </c>
@@ -1693,7 +1692,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="14.4">
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" s="35" t="s">
         <v>69</v>
       </c>
@@ -1713,13 +1712,13 @@
         <v>44548</v>
       </c>
       <c r="G29" s="10">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="14.4">
+    <row r="30" spans="1:11" ht="15">
       <c r="A30" s="35" t="s">
         <v>46</v>
       </c>
@@ -1735,13 +1734,13 @@
         <v>44550</v>
       </c>
       <c r="G30" s="10">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="14.4">
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="45" t="s">
         <v>73</v>
       </c>
@@ -1765,7 +1764,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="14.4">
+    <row r="32" spans="1:11" ht="15">
       <c r="A32" s="46"/>
       <c r="B32" s="42" t="s">
         <v>118</v>
@@ -1783,7 +1782,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="14.4">
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1795,7 +1794,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="14.4">
+    <row r="34" spans="1:11" ht="15">
       <c r="C34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1805,7 +1804,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="14.4">
+    <row r="35" spans="1:11" ht="15">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1814,13 +1813,13 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="14.4">
+    <row r="36" spans="1:11" ht="15">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="14.4">
+    <row r="37" spans="1:11" ht="15">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1829,7 +1828,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="14.4">
+    <row r="38" spans="1:11" ht="15">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1838,7 +1837,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="14.4">
+    <row r="39" spans="1:11" ht="15">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1847,7 +1846,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="14.4">
+    <row r="40" spans="1:11" ht="15">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1856,7 +1855,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="14.4">
+    <row r="41" spans="1:11" ht="15">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -1865,7 +1864,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="14.4">
+    <row r="42" spans="1:11" ht="15">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1958,7 +1957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1968,14 +1967,14 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.8">
+    <row r="1" spans="1:4" ht="14.25">
       <c r="A1" s="51" t="s">
         <v>74</v>
       </c>

</xml_diff>